<commit_message>
addded normal XLS, XLSX for downloading them from server
</commit_message>
<xml_diff>
--- a/server/files/template.xlsx
+++ b/server/files/template.xlsx
@@ -2,39 +2,229 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+  <workbookPr defaultThemeVersion="164011"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Ubuntu\Evotor\Helper\server\files\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="993"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="0" iterateDelta="1E-4"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
+    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
+      <loext:extCalcPr stringRefSyntax="ExcelA1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
-  <si>
-    <t>Тест</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Название товара
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>(обязательное поле)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Код товара
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>(до 10 символов)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Артикул</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> 
+(до 20 символов)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Штрихкоды</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">  
+(Если оставить штрихкоды пустыми, в терминале будет доступен только визуальный поиск товара)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Отпускная цена</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> (обязательное поле)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Закупочная цена
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>(обязательное поле)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Ставка НДС 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>(два символа через пробел: 
+% (0 – Без НДС)
+“с” - “с рачсетной ставкой”/”н” - “Без”)</t>
+    </r>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>Пример</t>
+  </si>
+  <si>
+    <t>Артикул123456789</t>
+  </si>
+  <si>
+    <t>Какой-то штрихкод</t>
+  </si>
+  <si>
+    <t>18.00</t>
+  </si>
+  <si>
+    <t>123.20</t>
+  </si>
+  <si>
+    <t>0 б</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -57,8 +247,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -339,29 +535,76 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="27.7109375"/>
+    <col min="2" max="2" width="20.28515625"/>
+    <col min="3" max="3" width="23.7109375"/>
+    <col min="4" max="4" width="38.28515625"/>
+    <col min="5" max="5" width="17"/>
+    <col min="6" max="6" width="16"/>
+    <col min="7" max="7" width="31.140625"/>
+    <col min="8" max="1025" width="8.5703125"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:9" ht="57" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1">
+      <c r="D1" s="1" t="s">
         <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="2"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2">
+        <v>1234567890</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
</xml_diff>